<commit_message>
Agregando primer version del cartel para presentacion de aplicaicon de modelos de pronostico a demanda_electrico
</commit_message>
<xml_diff>
--- a/Demanda_electrico_2022_full1 - Copy.xlsx
+++ b/Demanda_electrico_2022_full1 - Copy.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9e6e0322c927b48/Documentos/MIS_UNAM/Segundo_semestre/Pronosticos_UNAM_HPi3/pronosticos_UNAM_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BACC65B0-C542-4DF3-975D-0BB62EAD5A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:40009_{BACC65B0-C542-4DF3-975D-0BB62EAD5A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D0A49A7-AC04-4CF7-8A1B-199BC8FA53C8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="7284" yWindow="960" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demanda_electrico_2022_full1 - " sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2708,16 +2708,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>193</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>338846</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>36074</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>208</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>232167</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>36075</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3041,11 +3041,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A214" sqref="A214"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="119" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>